<commit_message>
Beispiel 8 komplett validiert und Verbesserungen
</commit_message>
<xml_diff>
--- a/data/Beispiel_8a.xlsx
+++ b/data/Beispiel_8a.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e1d3018db502cb77/Documents/GitHub/Kurzschlussfestigkeit/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{79E52F01-784B-41D3-AFAA-C73478ADE294}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{561A9464-CCCD-4C21-B970-DABD200DC29A}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{79E52F01-784B-41D3-AFAA-C73478ADE294}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{79908751-D431-4E18-A498-21AEFF35FC19}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -183,10 +183,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="12">
+  <numFmts count="11">
     <numFmt numFmtId="164" formatCode="#,##0.0\ &quot;MVA&quot;"/>
     <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;m&quot;"/>
-    <numFmt numFmtId="166" formatCode="#,##0.0"/>
     <numFmt numFmtId="167" formatCode="##0\ &quot;°C&quot;"/>
     <numFmt numFmtId="168" formatCode="#,##0.0\ &quot;kA&quot;"/>
     <numFmt numFmtId="169" formatCode="#,##0.0\ &quot;s&quot;"/>
@@ -731,9 +730,6 @@
     <xf numFmtId="165" fontId="11" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="11" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="3" fontId="11" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -781,19 +777,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="11" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="12" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="11" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -803,8 +790,20 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="12" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="11" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="12" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="12" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="11" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="11" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="14">
@@ -1042,7 +1041,7 @@
   <dimension ref="A1:F72"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScale="145" zoomScaleNormal="145" zoomScaleSheetLayoutView="130" zoomScalePageLayoutView="145" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.75" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -1072,19 +1071,19 @@
       <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:6" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="43"/>
+      <c r="B3" s="42"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="44" t="s">
+      <c r="A4" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="45"/>
+      <c r="B4" s="44"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -1093,7 +1092,7 @@
       <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="36" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="1"/>
@@ -1105,7 +1104,7 @@
       <c r="A6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="38" t="s">
+      <c r="B6" s="37" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="1"/>
@@ -1117,7 +1116,7 @@
       <c r="A7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="38" t="s">
+      <c r="B7" s="37" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="1"/>
@@ -1129,7 +1128,7 @@
       <c r="A8" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="38"/>
+      <c r="B8" s="37"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -1139,7 +1138,7 @@
       <c r="A9" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="30">
+      <c r="B9" s="29">
         <v>-20</v>
       </c>
     </row>
@@ -1147,21 +1146,21 @@
       <c r="A10" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="31">
+      <c r="B10" s="30">
         <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="40" t="s">
+      <c r="A11" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="41"/>
+      <c r="B11" s="40"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="32">
+      <c r="B12" s="31">
         <v>63</v>
       </c>
     </row>
@@ -1169,15 +1168,15 @@
       <c r="A13" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="28">
-        <v>1.8</v>
+      <c r="B13" s="54">
+        <v>1.81</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="33">
+      <c r="B14" s="32">
         <v>0.5</v>
       </c>
     </row>
@@ -1185,21 +1184,21 @@
       <c r="A15" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B15" s="39">
+      <c r="B15" s="38">
         <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="40" t="s">
+      <c r="A16" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="41"/>
+      <c r="B16" s="40"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="37" t="s">
+      <c r="B17" s="36" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1207,7 +1206,7 @@
       <c r="A18" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="29">
+      <c r="B18" s="28">
         <v>2</v>
       </c>
     </row>
@@ -1215,15 +1214,15 @@
       <c r="A19" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="34">
+      <c r="B19" s="33">
         <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="40" t="s">
+      <c r="A20" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="41"/>
+      <c r="B20" s="40"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
@@ -1258,16 +1257,16 @@
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="40" t="s">
+      <c r="A25" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="B25" s="41"/>
+      <c r="B25" s="40"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="35">
+      <c r="B26" s="34">
         <v>17.8</v>
       </c>
     </row>
@@ -1275,7 +1274,7 @@
       <c r="A27" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="35">
+      <c r="B27" s="34">
         <v>15.4</v>
       </c>
     </row>
@@ -1283,15 +1282,15 @@
       <c r="A28" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B28" s="36">
+      <c r="B28" s="35">
         <v>500000</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="40" t="s">
+      <c r="A29" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="B29" s="41"/>
+      <c r="B29" s="40"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
@@ -1585,10 +1584,10 @@
     </row>
     <row r="2" spans="1:6" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:6" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="43"/>
+      <c r="B3" s="42"/>
       <c r="C3" s="10" t="s">
         <v>43</v>
       </c>
@@ -1603,10 +1602,10 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="54" t="s">
+      <c r="A4" s="52" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="45"/>
+      <c r="B4" s="44"/>
       <c r="C4" s="12" t="s">
         <v>48</v>
       </c>
@@ -1621,106 +1620,106 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="47" t="s">
+      <c r="A5" s="50" t="s">
         <v>50</v>
       </c>
-      <c r="B5" s="41"/>
+      <c r="B5" s="40"/>
       <c r="C5" s="16"/>
       <c r="D5" s="17"/>
       <c r="E5" s="17"/>
       <c r="F5" s="18"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="48"/>
-      <c r="B6" s="41"/>
+      <c r="A6" s="51"/>
+      <c r="B6" s="40"/>
       <c r="C6" s="19"/>
       <c r="D6" s="20"/>
       <c r="E6" s="20"/>
       <c r="F6" s="21"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="47"/>
-      <c r="B7" s="41"/>
+      <c r="A7" s="50"/>
+      <c r="B7" s="40"/>
       <c r="C7" s="16"/>
       <c r="D7" s="17"/>
       <c r="E7" s="17"/>
       <c r="F7" s="18"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="48"/>
-      <c r="B8" s="41"/>
+      <c r="A8" s="51"/>
+      <c r="B8" s="40"/>
       <c r="C8" s="19"/>
       <c r="D8" s="20"/>
       <c r="E8" s="20"/>
       <c r="F8" s="21"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="47"/>
-      <c r="B9" s="41"/>
+      <c r="A9" s="50"/>
+      <c r="B9" s="40"/>
       <c r="C9" s="16"/>
       <c r="D9" s="17"/>
       <c r="E9" s="17"/>
       <c r="F9" s="18"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="48"/>
-      <c r="B10" s="41"/>
+      <c r="A10" s="51"/>
+      <c r="B10" s="40"/>
       <c r="C10" s="19"/>
       <c r="D10" s="20"/>
       <c r="E10" s="20"/>
       <c r="F10" s="21"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="47"/>
-      <c r="B11" s="41"/>
+      <c r="A11" s="50"/>
+      <c r="B11" s="40"/>
       <c r="C11" s="16"/>
       <c r="D11" s="17"/>
       <c r="E11" s="17"/>
       <c r="F11" s="18"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="53"/>
-      <c r="B12" s="41"/>
+      <c r="A12" s="49"/>
+      <c r="B12" s="40"/>
       <c r="C12" s="19"/>
       <c r="D12" s="20"/>
       <c r="E12" s="20"/>
       <c r="F12" s="21"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="49"/>
-      <c r="B13" s="41"/>
+      <c r="A13" s="53"/>
+      <c r="B13" s="40"/>
       <c r="C13" s="16"/>
       <c r="D13" s="17"/>
       <c r="E13" s="17"/>
       <c r="F13" s="18"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="48"/>
-      <c r="B14" s="41"/>
+      <c r="A14" s="51"/>
+      <c r="B14" s="40"/>
       <c r="C14" s="19"/>
       <c r="D14" s="20"/>
       <c r="E14" s="20"/>
       <c r="F14" s="21"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="47"/>
-      <c r="B15" s="41"/>
+      <c r="A15" s="50"/>
+      <c r="B15" s="40"/>
       <c r="C15" s="16"/>
       <c r="D15" s="17"/>
       <c r="E15" s="17"/>
       <c r="F15" s="18"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="48"/>
-      <c r="B16" s="41"/>
+      <c r="A16" s="51"/>
+      <c r="B16" s="40"/>
       <c r="C16" s="19"/>
       <c r="D16" s="20"/>
       <c r="E16" s="20"/>
       <c r="F16" s="21"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="47"/>
-      <c r="B17" s="41"/>
+      <c r="A17" s="50"/>
+      <c r="B17" s="40"/>
       <c r="C17" s="16"/>
       <c r="D17" s="17"/>
       <c r="E17" s="17"/>
@@ -1728,15 +1727,15 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="46"/>
-      <c r="B18" s="41"/>
+      <c r="B18" s="40"/>
       <c r="C18" s="19"/>
       <c r="D18" s="20"/>
       <c r="E18" s="20"/>
       <c r="F18" s="21"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="50"/>
-      <c r="B19" s="41"/>
+      <c r="A19" s="45"/>
+      <c r="B19" s="40"/>
       <c r="C19" s="16"/>
       <c r="D19" s="17"/>
       <c r="E19" s="17"/>
@@ -1744,15 +1743,15 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="46"/>
-      <c r="B20" s="41"/>
+      <c r="B20" s="40"/>
       <c r="C20" s="19"/>
       <c r="D20" s="20"/>
       <c r="E20" s="20"/>
       <c r="F20" s="21"/>
     </row>
     <row r="21" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="50"/>
-      <c r="B21" s="41"/>
+      <c r="A21" s="45"/>
+      <c r="B21" s="40"/>
       <c r="C21" s="16"/>
       <c r="D21" s="17"/>
       <c r="E21" s="17"/>
@@ -1760,15 +1759,15 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="46"/>
-      <c r="B22" s="41"/>
+      <c r="B22" s="40"/>
       <c r="C22" s="19"/>
       <c r="D22" s="20"/>
       <c r="E22" s="20"/>
       <c r="F22" s="21"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="50"/>
-      <c r="B23" s="41"/>
+      <c r="A23" s="45"/>
+      <c r="B23" s="40"/>
       <c r="C23" s="16"/>
       <c r="D23" s="17"/>
       <c r="E23" s="17"/>
@@ -1776,15 +1775,15 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="46"/>
-      <c r="B24" s="41"/>
+      <c r="B24" s="40"/>
       <c r="C24" s="19"/>
       <c r="D24" s="20"/>
       <c r="E24" s="20"/>
       <c r="F24" s="21"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="50"/>
-      <c r="B25" s="41"/>
+      <c r="A25" s="45"/>
+      <c r="B25" s="40"/>
       <c r="C25" s="16"/>
       <c r="D25" s="17"/>
       <c r="E25" s="17"/>
@@ -1792,15 +1791,15 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="46"/>
-      <c r="B26" s="41"/>
+      <c r="B26" s="40"/>
       <c r="C26" s="19"/>
       <c r="D26" s="20"/>
       <c r="E26" s="20"/>
       <c r="F26" s="21"/>
     </row>
     <row r="27" spans="1:6" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="51"/>
-      <c r="B27" s="52"/>
+      <c r="A27" s="47"/>
+      <c r="B27" s="48"/>
       <c r="C27" s="22"/>
       <c r="D27" s="23"/>
       <c r="E27" s="23"/>
@@ -1809,6 +1808,15 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="L3JGn++vkSXlWLsCCYWWINtqUqmHh3ss+Y3UnfzvYnEO110ZTLt4h5Wk1J0P8sdh9gATNb+6gDKHOpRAIsir+Q==" saltValue="aQCLb7ecvUo3cSUIR9a0KA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="25">
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A9:B9"/>
     <mergeCell ref="A25:B25"/>
     <mergeCell ref="A18:B18"/>
     <mergeCell ref="A27:B27"/>
@@ -1825,15 +1833,6 @@
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A9:B9"/>
   </mergeCells>
   <pageMargins left="0.78740157480314965" right="0.55118110236220474" top="1.181102362204725" bottom="0.9055118110236221" header="0.47244094488188981" footer="0.35433070866141742"/>
   <pageSetup paperSize="9" pageOrder="overThenDown" orientation="portrait" r:id="rId1"/>

</xml_diff>